<commit_message>
todas las funcionalidades menos los radioitem
</commit_message>
<xml_diff>
--- a/datos - copia.xlsx
+++ b/datos - copia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geo\eclipse-workspace\cotizador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12789F23-FE93-4565-B5C5-7EA9C2F2B34D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DE5679-ADD5-44F3-87F0-21691D4E6EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{BFD0BB4B-DE68-4FA6-B1E7-517AB002CC00}"/>
+    <workbookView minimized="1" xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="6" xr2:uid="{BFD0BB4B-DE68-4FA6-B1E7-517AB002CC00}"/>
   </bookViews>
   <sheets>
     <sheet name="Semi" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Extensible" sheetId="4" r:id="rId4"/>
     <sheet name="Modulo hidraulico" sheetId="6" r:id="rId5"/>
     <sheet name="Acompa" sheetId="1" r:id="rId6"/>
+    <sheet name="permiso" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="203">
   <si>
     <t>sfm30</t>
   </si>
@@ -627,6 +628,18 @@
   </si>
   <si>
     <t>Ext20t18m365x380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permiso bs as </t>
+  </si>
+  <si>
+    <t>p caba</t>
+  </si>
+  <si>
+    <t>p neuquen</t>
+  </si>
+  <si>
+    <t>p sta cruz</t>
   </si>
 </sst>
 </file>
@@ -1905,7 +1918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C83BBA-CD1E-42A8-8501-9CE20F523C50}">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3067,4 +3080,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8C7C8A-FAB0-4AD2-B6A4-BB5B42A89115}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>